<commit_message>
fix : updated excel
</commit_message>
<xml_diff>
--- a/evolution.xlsx
+++ b/evolution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Bureau\EFREI\Semestre 10\kata-contacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2899A8EC-5A77-43C6-A4B8-257F14DC3BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B43A8AA0-271C-4F51-8752-2F8F6D213DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F610E1FF-3040-4D26-A9ED-8663A0A3C9AA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>size</t>
   </si>
@@ -197,6 +197,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Sans index</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -273,6 +276,61 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A240-497A-B6A7-F84002CC19F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Avec index</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$F$6:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AEDB-41C3-9473-E54503D96A05}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -518,6 +576,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1128,10 +1217,10 @@
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1456,76 +1545,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A555143-AC8E-4AE4-8BF3-EED362C07594}">
-  <dimension ref="D5:E12"/>
+  <dimension ref="D5:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D6" s="1">
         <v>10</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
       </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D7" s="1">
         <v>100</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
       </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D8" s="1">
         <v>1000</v>
       </c>
       <c r="E8" s="1">
         <v>1.0009999999999999</v>
       </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D9" s="1">
         <v>10000</v>
       </c>
       <c r="E9" s="1">
         <v>2.0059999999999998</v>
       </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D10" s="1">
         <v>50000</v>
       </c>
       <c r="E10" s="1">
         <v>14.997</v>
       </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D11" s="1">
         <v>100000</v>
       </c>
       <c r="E11" s="1">
         <v>23.998999999999999</v>
       </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D12" s="1">
         <v>1000000</v>
       </c>
       <c r="E12" s="1">
         <v>272.017</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>